<commit_message>
Commit avant changement controlModelInfo
</commit_message>
<xml_diff>
--- a/SonarLysaFX/src/test/resources/Suivi_Quality_Gate - DataStageTest.xlsx
+++ b/SonarLysaFX/src/test/resources/Suivi_Quality_Gate - DataStageTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="136">
   <si>
     <t>Edition</t>
   </si>
@@ -1384,6 +1384,45 @@
   </si>
   <si>
     <t>Informations d'utilisation du fichier</t>
+  </si>
+  <si>
+    <t>NPC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- NPC : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Indique si le projet est un projet NPC - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Origine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : fichier Excel NPC</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2679,10 +2718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T82"/>
+  <dimension ref="A2:T83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,66 +3084,71 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="88" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="88" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="88" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="88" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="88" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="88" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="88" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="88" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="88" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="88" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="88" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="88" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="20:20" x14ac:dyDescent="0.25">
-      <c r="T82" s="87" t="s">
+    <row r="83" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T83" s="87" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3285,9 +3329,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3302,21 +3348,22 @@
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="41" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="90.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="90.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -3350,44 +3397,47 @@
       <c r="K1" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="Q1" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="R1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="S1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="T1" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="U1" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="V1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="W1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="X1" s="36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>64</v>
       </c>
@@ -3421,38 +3471,39 @@
       <c r="K2" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="62">
+      <c r="L2" s="84"/>
+      <c r="M2" s="62">
         <v>43138</v>
       </c>
-      <c r="M2" s="61" t="s">
+      <c r="N2" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="N2" s="64">
+      <c r="O2" s="64">
         <v>312996</v>
-      </c>
-      <c r="O2" s="61" t="s">
-        <v>37</v>
       </c>
       <c r="P2" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62">
+      <c r="Q2" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62">
         <v>43168</v>
       </c>
-      <c r="S2" s="62"/>
       <c r="T2" s="62"/>
-      <c r="U2" s="60" t="s">
+      <c r="U2" s="62"/>
+      <c r="V2" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="V2" s="60" t="s">
+      <c r="W2" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="W2" s="61" t="s">
+      <c r="X2" s="61" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>64</v>
       </c>
@@ -3486,38 +3537,39 @@
       <c r="K3" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="L3" s="67">
+      <c r="L3" s="84"/>
+      <c r="M3" s="67">
         <v>43214</v>
       </c>
-      <c r="M3" s="66" t="s">
+      <c r="N3" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="69">
+      <c r="O3" s="69">
         <v>313058</v>
-      </c>
-      <c r="O3" s="66" t="s">
-        <v>37</v>
       </c>
       <c r="P3" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67">
+      <c r="Q3" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67">
         <v>43168</v>
       </c>
-      <c r="S3" s="67"/>
       <c r="T3" s="67"/>
-      <c r="U3" s="65" t="s">
+      <c r="U3" s="67"/>
+      <c r="V3" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="V3" s="65" t="s">
+      <c r="W3" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="W3" s="66" t="s">
+      <c r="X3" s="66" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
         <v>42</v>
       </c>
@@ -3551,38 +3603,39 @@
       <c r="K4" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="72">
+      <c r="L4" s="84"/>
+      <c r="M4" s="72">
         <v>43153</v>
       </c>
-      <c r="M4" s="71" t="s">
+      <c r="N4" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="N4" s="74">
+      <c r="O4" s="74">
         <v>312946</v>
       </c>
-      <c r="O4" s="71" t="s">
+      <c r="P4" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="71" t="s">
+      <c r="Q4" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72">
+      <c r="R4" s="72"/>
+      <c r="S4" s="72">
         <v>43168</v>
       </c>
-      <c r="S4" s="72"/>
       <c r="T4" s="72"/>
-      <c r="U4" s="70" t="s">
+      <c r="U4" s="72"/>
+      <c r="V4" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="V4" s="70" t="s">
+      <c r="W4" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="W4" s="71" t="s">
+      <c r="X4" s="71" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="75" t="s">
         <v>42</v>
       </c>
@@ -3616,34 +3669,35 @@
       <c r="K5" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="77">
+      <c r="L5" s="84"/>
+      <c r="M5" s="77">
         <v>43129</v>
       </c>
-      <c r="M5" s="76" t="s">
+      <c r="N5" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76" t="s">
-        <v>37</v>
-      </c>
+      <c r="O5" s="76"/>
       <c r="P5" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="Q5" s="77"/>
+      <c r="Q5" s="76" t="s">
+        <v>37</v>
+      </c>
       <c r="R5" s="77"/>
       <c r="S5" s="77"/>
       <c r="T5" s="77"/>
-      <c r="U5" s="75" t="s">
+      <c r="U5" s="77"/>
+      <c r="V5" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="V5" s="75" t="s">
+      <c r="W5" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="W5" s="76" t="s">
+      <c r="X5" s="76" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>42</v>
       </c>
@@ -3677,34 +3731,35 @@
       <c r="K6" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="L6" s="81">
+      <c r="L6" s="84"/>
+      <c r="M6" s="81">
         <v>43130</v>
       </c>
-      <c r="M6" s="80" t="s">
+      <c r="N6" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80" t="s">
-        <v>37</v>
-      </c>
+      <c r="O6" s="80"/>
       <c r="P6" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="81"/>
+      <c r="Q6" s="80" t="s">
+        <v>37</v>
+      </c>
       <c r="R6" s="81"/>
       <c r="S6" s="81"/>
       <c r="T6" s="81"/>
-      <c r="U6" s="79" t="s">
+      <c r="U6" s="81"/>
+      <c r="V6" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="V6" s="79" t="s">
+      <c r="W6" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="W6" s="80" t="s">
+      <c r="X6" s="80" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="83" t="s">
         <v>69</v>
       </c>
@@ -3738,44 +3793,45 @@
       <c r="K7" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="85"/>
-      <c r="M7" s="84" t="s">
+      <c r="L7" s="84"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84" t="s">
-        <v>37</v>
-      </c>
+      <c r="O7" s="84"/>
       <c r="P7" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="Q7" s="85"/>
+      <c r="Q7" s="84" t="s">
+        <v>37</v>
+      </c>
       <c r="R7" s="85"/>
       <c r="S7" s="85"/>
       <c r="T7" s="85"/>
-      <c r="U7" s="83" t="s">
+      <c r="U7" s="85"/>
+      <c r="V7" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="83" t="s">
+      <c r="W7" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="W7" s="84" t="s">
+      <c r="X7" s="84" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Erreur Action" error="Valeur pour l'action interdite" sqref="P2:P7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Erreur Action" error="Valeur pour l'action interdite" sqref="Q2:Q7">
       <formula1>"A créer,A vérifier,,A assembler,A clôturer,A abandonner"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="N2" r:id="rId2" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=312996" display="https://ttp10-jazz.ca-technologies.credit-agricole.fr/ccm/web/projects/PRJF_BFCC20_MKT_Comm client Etape 2 - action=com.ibm.team.workitem.viewWorkItem&amp;id=312996"/>
+    <hyperlink ref="O2" r:id="rId2" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=312996" display="https://ttp10-jazz.ca-technologies.credit-agricole.fr/ccm/web/projects/PRJF_BFCC20_MKT_Comm client Etape 2 - action=com.ibm.team.workitem.viewWorkItem&amp;id=312996"/>
     <hyperlink ref="I3" r:id="rId3"/>
-    <hyperlink ref="N3" r:id="rId4" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=313058" display="https://ttp10-jazz.ca-technologies.credit-agricole.fr/ccm/web/projects/PRJM_FE000062_Coclico_Données - action=com.ibm.team.workitem.viewWorkItem&amp;id=313058"/>
+    <hyperlink ref="O3" r:id="rId4" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=313058" display="https://ttp10-jazz.ca-technologies.credit-agricole.fr/ccm/web/projects/PRJM_FE000062_Coclico_Données - action=com.ibm.team.workitem.viewWorkItem&amp;id=313058"/>
     <hyperlink ref="I4" r:id="rId5"/>
-    <hyperlink ref="N4" r:id="rId6" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=312946" display="https://ttp10-jazz.ca-technologies.credit-agricole.fr/ccm/web/projects/PRJF_BF0548_MKT_Rempl outil envoi Emails - action=com.ibm.team.workitem.viewWorkItem&amp;id=312946"/>
+    <hyperlink ref="O4" r:id="rId6" location="action=com.ibm.team.workitem.viewWorkItem&amp;id=312946" display="https://ttp10-jazz.ca-technologies.credit-agricole.fr/ccm/web/projects/PRJF_BF0548_MKT_Rempl outil envoi Emails - action=com.ibm.team.workitem.viewWorkItem&amp;id=312946"/>
     <hyperlink ref="I5" r:id="rId7"/>
     <hyperlink ref="I6" r:id="rId8"/>
     <hyperlink ref="I7" r:id="rId9"/>
@@ -3786,9 +3842,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3802,21 +3860,22 @@
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
@@ -3850,40 +3909,43 @@
       <c r="K1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="N1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="O1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="P1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="Q1" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="R1" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="54" t="s">
+      <c r="S1" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="T1" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="U1" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="57" t="s">
+      <c r="V1" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="58" t="s">
+      <c r="W1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="59" t="s">
+      <c r="X1" s="59" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>